<commit_message>
Actualizaciones UI y dashboard
</commit_message>
<xml_diff>
--- a/public/templates/plantilla-importacion-productos.xlsx
+++ b/public/templates/plantilla-importacion-productos.xlsx
@@ -397,10 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -422,40 +425,46 @@
         <v>STOCK *</v>
       </c>
       <c r="G1" t="str">
+        <v>STOCK MINIMO</v>
+      </c>
+      <c r="H1" t="str">
         <v>CATEGORIA</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>DESCRIPCION</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>IMAGEN (URL o data)</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>FECHA VENCIMIENTO (YYYY-MM-DD)</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>VARIANTE NOMBRE (OPCIONAL)</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>VARIANTE CODIGO (OPCIONAL)</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>VARIANTE STOCK (OPCIONAL)</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>MARCA</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>MODELO</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>COLOR</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>TALLA</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>MATERIAL</v>
+      </c>
+      <c r="T1" t="str">
+        <v>PERMITE TOPPINGS (SI/NO)</v>
       </c>
     </row>
     <row r="2">
@@ -477,15 +486,15 @@
       <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="str">
         <v>Ropa</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>Camisa de algodÃ³n 100% color azul marino talla M</v>
       </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
       <c r="J2" t="str">
         <v/>
       </c>
@@ -499,19 +508,25 @@
         <v/>
       </c>
       <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
         <v>MarcaX</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <v>Modelo-Polo</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>Azul</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <v>M</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <v>AlgodÃ³n</v>
+      </c>
+      <c r="T2" t="str">
+        <v>no</v>
       </c>
     </row>
     <row r="3">
@@ -533,41 +548,47 @@
       <c r="F3" t="str">
         <v/>
       </c>
-      <c r="G3" t="str">
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="str">
         <v>CosmÃ©tica</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>Base lÃ­quida para rostro</v>
       </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
       <c r="J3" t="str">
         <v/>
       </c>
       <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
         <v>Tono 01</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <v>SKU-003-T01</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>12</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <v>MarcaY</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <v>BasePro</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <v>Tono 01</v>
       </c>
-      <c r="Q3" t="str">
-        <v/>
-      </c>
       <c r="R3" t="str">
         <v/>
+      </c>
+      <c r="S3" t="str">
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <v>no</v>
       </c>
     </row>
     <row r="4">
@@ -589,41 +610,47 @@
       <c r="F4" t="str">
         <v/>
       </c>
-      <c r="G4" t="str">
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" t="str">
         <v>CosmÃ©tica</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>Base lÃ­quida para rostro</v>
       </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
       <c r="J4" t="str">
         <v/>
       </c>
       <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
         <v>Tono 02</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <v>SKU-003-T02</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>8</v>
       </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
         <v>MarcaY</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <v>BasePro</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <v>Tono 02</v>
       </c>
-      <c r="Q4" t="str">
-        <v/>
-      </c>
       <c r="R4" t="str">
         <v/>
+      </c>
+      <c r="S4" t="str">
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <v>no</v>
       </c>
     </row>
     <row r="5">
@@ -645,15 +672,15 @@
       <c r="F5" t="str">
         <v/>
       </c>
-      <c r="G5" t="str">
-        <v/>
+      <c r="G5">
+        <v>8</v>
       </c>
       <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
         <v>Servicio de manicure</v>
       </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
       <c r="J5" t="str">
         <v/>
       </c>
@@ -677,11 +704,17 @@
       </c>
       <c r="Q5" t="str">
         <v/>
+      </c>
+      <c r="R5" t="str">
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <v>no</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>